<commit_message>
PR updated to include categories; remains without implementation options
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_PR.xlsx
+++ b/curation/draft/collection/collection_specialization_PR.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B16D7F7-37E7-42B3-A5A3-E12960AC2D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F53AE-2878-F749-ABC2-8D2ECFE7D296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_PR" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_PR!$A$1:$AI$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_PR!$A$1:$AJ$60</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
@@ -490,13 +490,13 @@
     <t>PR_SHORT</t>
   </si>
   <si>
-    <t>LZZT - 360i</t>
-  </si>
-  <si>
     <t>NOT DONE</t>
   </si>
   <si>
     <t>PR_SHORT_360</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -879,33 +879,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG60"/>
+  <dimension ref="A1:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="H61" sqref="H61"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="5"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="15" max="15" width="32.140625" customWidth="1"/>
-    <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="25" max="25" width="19.85546875" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" customWidth="1"/>
-    <col min="28" max="28" width="17" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" customWidth="1"/>
-    <col min="31" max="31" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="31.5" customWidth="1"/>
+    <col min="12" max="12" width="26.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" customWidth="1"/>
+    <col min="16" max="16" width="32.1640625" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" customWidth="1"/>
+    <col min="26" max="26" width="19.83203125" customWidth="1"/>
+    <col min="27" max="27" width="14.83203125" customWidth="1"/>
+    <col min="29" max="29" width="17" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" customWidth="1"/>
+    <col min="32" max="32" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,77 +936,80 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>150</v>
       </c>
@@ -1022,47 +1025,47 @@
       <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>36</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>41</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>150</v>
       </c>
@@ -1078,35 +1081,35 @@
       <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="L3" t="s">
-        <v>151</v>
       </c>
       <c r="M3" t="s">
         <v>151</v>
       </c>
-      <c r="P3" t="s">
+      <c r="N3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" t="s">
         <v>152</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>67</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>10</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>153</v>
       </c>
       <c r="AE3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>43</v>
       </c>
@@ -1125,44 +1128,44 @@
       <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" t="s">
-        <v>46</v>
       </c>
       <c r="M4" t="s">
         <v>46</v>
       </c>
       <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
         <v>47</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>48</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>49</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>36</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>200</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>137</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>46</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -1181,41 +1184,41 @@
       <c r="H5" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L5" t="s">
-        <v>50</v>
       </c>
       <c r="M5" t="s">
         <v>50</v>
       </c>
       <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
         <v>51</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>52</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>49</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>36</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>200</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>50</v>
       </c>
       <c r="AE5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>43</v>
       </c>
@@ -1234,53 +1237,53 @@
       <c r="H6" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L6" t="s">
-        <v>53</v>
       </c>
       <c r="M6" t="s">
         <v>53</v>
       </c>
       <c r="N6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s">
         <v>54</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>55</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>56</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>36</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>200</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>138</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>139</v>
       </c>
-      <c r="AB6" s="6" t="s">
+      <c r="AC6" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>43</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>53</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>43</v>
       </c>
@@ -1299,56 +1302,56 @@
       <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
       </c>
       <c r="M7" t="s">
         <v>57</v>
       </c>
       <c r="N7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" t="s">
         <v>58</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>59</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>49</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>36</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>1</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>56</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>37</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>38</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>56</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>145</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>57</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1367,56 +1370,56 @@
       <c r="H8" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L8" t="s">
-        <v>60</v>
       </c>
       <c r="M8" t="s">
         <v>60</v>
       </c>
       <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
         <v>61</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>62</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>5</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>49</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>36</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>1</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>37</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>38</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>39</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>40</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>41</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>60</v>
       </c>
       <c r="AE8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>43</v>
       </c>
@@ -1435,41 +1438,41 @@
       <c r="H9" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>63</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>64</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>65</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>66</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>6</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>56</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>67</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>10</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>64</v>
       </c>
       <c r="AE9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -1488,41 +1491,41 @@
       <c r="H10" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>68</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>64</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>65</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>69</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>7</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>49</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>70</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>5</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>64</v>
       </c>
       <c r="AE10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -1541,56 +1544,56 @@
       <c r="H11" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L11" t="s">
-        <v>71</v>
       </c>
       <c r="M11" t="s">
         <v>71</v>
       </c>
       <c r="N11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" t="s">
         <v>72</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>73</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>49</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>36</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>200</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>56</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>74</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>75</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>76</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>77</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>71</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>78</v>
       </c>
@@ -1609,44 +1612,44 @@
       <c r="H12" t="s">
         <v>79</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L12" t="s">
-        <v>46</v>
       </c>
       <c r="M12" t="s">
         <v>46</v>
       </c>
       <c r="N12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" t="s">
         <v>47</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>48</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>1</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>49</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>36</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>200</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>137</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>46</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>78</v>
       </c>
@@ -1665,41 +1668,41 @@
       <c r="H13" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L13" t="s">
-        <v>50</v>
       </c>
       <c r="M13" t="s">
         <v>50</v>
       </c>
       <c r="N13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" t="s">
         <v>51</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>52</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>2</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>49</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>36</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>200</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>50</v>
       </c>
       <c r="AE13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>78</v>
       </c>
@@ -1718,53 +1721,53 @@
       <c r="H14" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L14" t="s">
-        <v>53</v>
       </c>
       <c r="M14" t="s">
         <v>53</v>
       </c>
       <c r="N14" t="s">
+        <v>53</v>
+      </c>
+      <c r="O14" t="s">
         <v>54</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>55</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>3</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>56</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>36</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>200</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>138</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>139</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>141</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>78</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>53</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>78</v>
       </c>
@@ -1783,56 +1786,56 @@
       <c r="H15" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L15" t="s">
-        <v>57</v>
       </c>
       <c r="M15" t="s">
         <v>57</v>
       </c>
       <c r="N15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O15" t="s">
         <v>58</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>59</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>4</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>49</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>36</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>1</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>56</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>37</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>38</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>56</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>145</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>57</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AF15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>78</v>
       </c>
@@ -1851,56 +1854,56 @@
       <c r="H16" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L16" t="s">
-        <v>60</v>
       </c>
       <c r="M16" t="s">
         <v>60</v>
       </c>
       <c r="N16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16" t="s">
         <v>61</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>81</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>5</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>49</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>36</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>1</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>37</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>38</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>39</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>40</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>41</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>60</v>
       </c>
       <c r="AE16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>78</v>
       </c>
@@ -1919,41 +1922,41 @@
       <c r="H17" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L17" t="s">
-        <v>63</v>
       </c>
       <c r="M17" t="s">
         <v>63</v>
       </c>
       <c r="N17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" t="s">
         <v>65</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>66</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>6</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>56</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>67</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>10</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>64</v>
       </c>
       <c r="AE17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>78</v>
       </c>
@@ -1972,41 +1975,41 @@
       <c r="H18" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L18" t="s">
-        <v>68</v>
       </c>
       <c r="M18" t="s">
         <v>68</v>
       </c>
       <c r="N18" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" t="s">
         <v>65</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>69</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>7</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>49</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>70</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>5</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>64</v>
       </c>
       <c r="AE18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>78</v>
       </c>
@@ -2025,56 +2028,56 @@
       <c r="H19" t="s">
         <v>79</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L19" t="s">
-        <v>71</v>
       </c>
       <c r="M19" t="s">
         <v>71</v>
       </c>
       <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" t="s">
         <v>72</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>73</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>8</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>49</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>36</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>200</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>56</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>74</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>75</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>82</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>83</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>71</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AF19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>84</v>
       </c>
@@ -2093,44 +2096,44 @@
       <c r="H20" t="s">
         <v>85</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L20" t="s">
-        <v>46</v>
       </c>
       <c r="M20" t="s">
         <v>46</v>
       </c>
       <c r="N20" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" t="s">
         <v>47</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>48</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>1</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>49</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>36</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>200</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>137</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>46</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AF20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>84</v>
       </c>
@@ -2149,41 +2152,41 @@
       <c r="H21" t="s">
         <v>85</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L21" t="s">
-        <v>50</v>
       </c>
       <c r="M21" t="s">
         <v>50</v>
       </c>
       <c r="N21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O21" t="s">
         <v>51</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>52</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>2</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>49</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>36</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>200</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>50</v>
       </c>
       <c r="AE21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>84</v>
       </c>
@@ -2202,53 +2205,53 @@
       <c r="H22" t="s">
         <v>85</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L22" t="s">
-        <v>53</v>
       </c>
       <c r="M22" t="s">
         <v>53</v>
       </c>
       <c r="N22" t="s">
+        <v>53</v>
+      </c>
+      <c r="O22" t="s">
         <v>54</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>55</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>3</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>56</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>36</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>200</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>138</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>139</v>
       </c>
-      <c r="AB22" s="6" t="s">
+      <c r="AC22" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="AC22" s="6" t="s">
+      <c r="AD22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>53</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AF22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>84</v>
       </c>
@@ -2267,56 +2270,56 @@
       <c r="H23" t="s">
         <v>85</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L23" t="s">
-        <v>57</v>
       </c>
       <c r="M23" t="s">
         <v>57</v>
       </c>
       <c r="N23" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" t="s">
         <v>58</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>59</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>4</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>49</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>36</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>1</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>56</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>37</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>38</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AC23" t="s">
         <v>56</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AD23" t="s">
         <v>145</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>57</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AF23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -2335,56 +2338,56 @@
       <c r="H24" t="s">
         <v>85</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L24" t="s">
-        <v>60</v>
       </c>
       <c r="M24" t="s">
         <v>60</v>
       </c>
       <c r="N24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" t="s">
         <v>61</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>87</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>5</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>49</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>36</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>1</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>37</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>38</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>39</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AA24" t="s">
         <v>40</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>41</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>60</v>
       </c>
       <c r="AE24" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>84</v>
       </c>
@@ -2403,41 +2406,41 @@
       <c r="H25" t="s">
         <v>85</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L25" t="s">
-        <v>63</v>
       </c>
       <c r="M25" t="s">
         <v>63</v>
       </c>
       <c r="N25" t="s">
+        <v>63</v>
+      </c>
+      <c r="O25" t="s">
         <v>65</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>66</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>6</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>56</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>67</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>10</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>64</v>
       </c>
       <c r="AE25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>84</v>
       </c>
@@ -2456,41 +2459,41 @@
       <c r="H26" t="s">
         <v>85</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L26" t="s">
-        <v>68</v>
       </c>
       <c r="M26" t="s">
         <v>68</v>
       </c>
       <c r="N26" t="s">
+        <v>68</v>
+      </c>
+      <c r="O26" t="s">
         <v>65</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>69</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>7</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>49</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>70</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>5</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>64</v>
       </c>
       <c r="AE26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>84</v>
       </c>
@@ -2509,56 +2512,56 @@
       <c r="H27" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L27" t="s">
-        <v>71</v>
       </c>
       <c r="M27" t="s">
         <v>71</v>
       </c>
       <c r="N27" t="s">
+        <v>71</v>
+      </c>
+      <c r="O27" t="s">
         <v>72</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>73</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>8</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>49</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>36</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>200</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>56</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>74</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>75</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AC27" t="s">
         <v>76</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AD27" t="s">
         <v>77</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>71</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AF27" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>88</v>
       </c>
@@ -2577,44 +2580,44 @@
       <c r="H28" t="s">
         <v>89</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="L28" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L28" t="s">
-        <v>46</v>
       </c>
       <c r="M28" t="s">
         <v>46</v>
       </c>
       <c r="N28" t="s">
+        <v>46</v>
+      </c>
+      <c r="O28" t="s">
         <v>47</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>48</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>1</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>49</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>36</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>200</v>
       </c>
-      <c r="AB28" t="s">
+      <c r="AC28" t="s">
         <v>91</v>
       </c>
-      <c r="AD28" t="s">
+      <c r="AE28" t="s">
         <v>46</v>
       </c>
-      <c r="AE28" t="s">
+      <c r="AF28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>88</v>
       </c>
@@ -2633,50 +2636,50 @@
       <c r="H29" t="s">
         <v>89</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="L29" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L29" t="s">
-        <v>50</v>
       </c>
       <c r="M29" t="s">
         <v>50</v>
       </c>
       <c r="N29" t="s">
+        <v>50</v>
+      </c>
+      <c r="O29" t="s">
         <v>51</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>52</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>2</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>49</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>36</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>200</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>92</v>
       </c>
-      <c r="Z29" t="s">
+      <c r="AA29" t="s">
         <v>93</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AB29" t="s">
         <v>41</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>50</v>
       </c>
       <c r="AE29" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AF29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>88</v>
       </c>
@@ -2695,44 +2698,44 @@
       <c r="H30" t="s">
         <v>89</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L30" t="s">
-        <v>94</v>
       </c>
       <c r="M30" t="s">
         <v>94</v>
       </c>
       <c r="N30" t="s">
+        <v>94</v>
+      </c>
+      <c r="O30" t="s">
         <v>95</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>96</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>3</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>49</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>36</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>200</v>
       </c>
-      <c r="AB30" t="s">
+      <c r="AC30" t="s">
         <v>97</v>
       </c>
-      <c r="AD30" t="s">
+      <c r="AE30" t="s">
         <v>94</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AF30" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>88</v>
       </c>
@@ -2751,56 +2754,56 @@
       <c r="H31" t="s">
         <v>89</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="L31" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L31" t="s">
-        <v>53</v>
       </c>
       <c r="M31" t="s">
         <v>53</v>
       </c>
       <c r="N31" t="s">
+        <v>53</v>
+      </c>
+      <c r="O31" t="s">
         <v>54</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>55</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>4</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>56</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>36</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>200</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>138</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Y31" t="s">
         <v>139</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>98</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="AA31" t="s">
         <v>99</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AB31" t="s">
         <v>41</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>53</v>
       </c>
       <c r="AE31" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AF31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>88</v>
       </c>
@@ -2819,56 +2822,56 @@
       <c r="H32" t="s">
         <v>89</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="L32" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L32" t="s">
-        <v>100</v>
       </c>
       <c r="M32" t="s">
         <v>100</v>
       </c>
       <c r="N32" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" t="s">
         <v>101</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>102</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>5</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>49</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>36</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>200</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>103</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>104</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>105</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AA32" t="s">
         <v>106</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>41</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AE32" t="s">
         <v>100</v>
       </c>
-      <c r="AE32" t="s">
+      <c r="AF32" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>88</v>
       </c>
@@ -2887,56 +2890,56 @@
       <c r="H33" t="s">
         <v>89</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L33" t="s">
-        <v>108</v>
       </c>
       <c r="M33" t="s">
         <v>108</v>
       </c>
       <c r="N33" t="s">
+        <v>108</v>
+      </c>
+      <c r="O33" t="s">
         <v>109</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>110</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>6</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>49</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>36</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>200</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>111</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>112</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>113</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="AA33" t="s">
         <v>114</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="AB33" t="s">
         <v>41</v>
       </c>
-      <c r="AD33" t="s">
+      <c r="AE33" t="s">
         <v>108</v>
       </c>
-      <c r="AE33" t="s">
+      <c r="AF33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>88</v>
       </c>
@@ -2955,56 +2958,56 @@
       <c r="H34" t="s">
         <v>89</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="L34" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L34" t="s">
-        <v>57</v>
       </c>
       <c r="M34" t="s">
         <v>57</v>
       </c>
       <c r="N34" t="s">
+        <v>57</v>
+      </c>
+      <c r="O34" t="s">
         <v>58</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>59</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>7</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>49</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>36</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>1</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>56</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>37</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>38</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AC34" t="s">
         <v>56</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AD34" t="s">
         <v>145</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AE34" t="s">
         <v>57</v>
       </c>
-      <c r="AE34" t="s">
+      <c r="AF34" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>88</v>
       </c>
@@ -3023,56 +3026,56 @@
       <c r="H35" t="s">
         <v>89</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="L35" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L35" t="s">
-        <v>60</v>
       </c>
       <c r="M35" t="s">
         <v>60</v>
       </c>
       <c r="N35" t="s">
+        <v>60</v>
+      </c>
+      <c r="O35" t="s">
         <v>61</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>116</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>8</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>49</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>36</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>1</v>
       </c>
-      <c r="W35" t="s">
+      <c r="X35" t="s">
         <v>37</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>38</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>39</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="AA35" t="s">
         <v>40</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AB35" t="s">
         <v>41</v>
-      </c>
-      <c r="AD35" t="s">
-        <v>60</v>
       </c>
       <c r="AE35" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AF35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>88</v>
       </c>
@@ -3091,41 +3094,41 @@
       <c r="H36" t="s">
         <v>89</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="L36" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L36" t="s">
-        <v>63</v>
       </c>
       <c r="M36" t="s">
         <v>63</v>
       </c>
       <c r="N36" t="s">
+        <v>63</v>
+      </c>
+      <c r="O36" t="s">
         <v>65</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>66</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
         <v>9</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>56</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>67</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>10</v>
-      </c>
-      <c r="AD36" t="s">
-        <v>64</v>
       </c>
       <c r="AE36" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AF36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -3144,38 +3147,38 @@
       <c r="H37" t="s">
         <v>89</v>
       </c>
-      <c r="K37" s="3" t="s">
+      <c r="L37" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L37" t="s">
-        <v>117</v>
       </c>
       <c r="M37" t="s">
         <v>117</v>
       </c>
-      <c r="P37" t="s">
+      <c r="N37" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q37" t="s">
         <v>118</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>10</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>56</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>36</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <v>100</v>
-      </c>
-      <c r="AD37" t="s">
-        <v>119</v>
       </c>
       <c r="AE37" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="38" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AF37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>88</v>
       </c>
@@ -3194,47 +3197,47 @@
       <c r="H38" t="s">
         <v>89</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="L38" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L38" t="s">
-        <v>120</v>
       </c>
       <c r="M38" t="s">
         <v>120</v>
       </c>
       <c r="N38" t="s">
+        <v>120</v>
+      </c>
+      <c r="O38" t="s">
         <v>121</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>122</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <v>11</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>56</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>36</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>20</v>
       </c>
-      <c r="AB38" t="s">
+      <c r="AC38" t="s">
         <v>123</v>
       </c>
-      <c r="AC38" t="s">
+      <c r="AD38" t="s">
         <v>124</v>
       </c>
-      <c r="AD38" t="s">
+      <c r="AE38" t="s">
         <v>120</v>
       </c>
-      <c r="AE38" t="s">
+      <c r="AF38" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>88</v>
       </c>
@@ -3253,41 +3256,41 @@
       <c r="H39" t="s">
         <v>89</v>
       </c>
-      <c r="K39" s="3" t="s">
+      <c r="L39" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L39" t="s">
-        <v>68</v>
       </c>
       <c r="M39" t="s">
         <v>68</v>
       </c>
       <c r="N39" t="s">
+        <v>68</v>
+      </c>
+      <c r="O39" t="s">
         <v>65</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>69</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <v>12</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>49</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>70</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>5</v>
-      </c>
-      <c r="AD39" t="s">
-        <v>64</v>
       </c>
       <c r="AE39" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AF39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -3306,56 +3309,56 @@
       <c r="H40" t="s">
         <v>89</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="L40" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L40" t="s">
-        <v>71</v>
       </c>
       <c r="M40" t="s">
         <v>71</v>
       </c>
       <c r="N40" t="s">
+        <v>71</v>
+      </c>
+      <c r="O40" t="s">
         <v>72</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>73</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <v>13</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>49</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>36</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>20</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>74</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>75</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>125</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="AA40" t="s">
         <v>126</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AB40" t="s">
         <v>41</v>
-      </c>
-      <c r="AD40" t="s">
-        <v>71</v>
       </c>
       <c r="AE40" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -3374,44 +3377,47 @@
       <c r="H41" t="s">
         <v>147</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="K41">
+        <v>360</v>
+      </c>
+      <c r="L41" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L41" t="s">
-        <v>46</v>
       </c>
       <c r="M41" t="s">
         <v>46</v>
       </c>
       <c r="N41" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" t="s">
         <v>47</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>48</v>
       </c>
-      <c r="Q41">
+      <c r="R41">
         <v>1</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>49</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>36</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <v>200</v>
       </c>
-      <c r="AB41" t="s">
+      <c r="AC41" t="s">
         <v>137</v>
       </c>
-      <c r="AD41" t="s">
+      <c r="AE41" t="s">
         <v>46</v>
       </c>
-      <c r="AE41" t="s">
+      <c r="AF41" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>43</v>
       </c>
@@ -3430,53 +3436,56 @@
       <c r="H42" t="s">
         <v>147</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="K42">
+        <v>360</v>
+      </c>
+      <c r="L42" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L42" t="s">
-        <v>53</v>
       </c>
       <c r="M42" t="s">
         <v>53</v>
       </c>
       <c r="N42" t="s">
+        <v>53</v>
+      </c>
+      <c r="O42" t="s">
         <v>54</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>55</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <v>3</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>56</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>36</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <v>200</v>
       </c>
-      <c r="W42" t="s">
+      <c r="X42" t="s">
         <v>138</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Y42" t="s">
         <v>139</v>
       </c>
-      <c r="AB42" s="6" t="s">
+      <c r="AC42" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AC42" t="s">
+      <c r="AD42" t="s">
         <v>43</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AE42" t="s">
         <v>53</v>
       </c>
-      <c r="AE42" t="s">
+      <c r="AF42" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>43</v>
       </c>
@@ -3495,56 +3504,59 @@
       <c r="H43" t="s">
         <v>147</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="K43">
+        <v>360</v>
+      </c>
+      <c r="L43" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L43" t="s">
-        <v>57</v>
       </c>
       <c r="M43" t="s">
         <v>57</v>
       </c>
       <c r="N43" t="s">
+        <v>57</v>
+      </c>
+      <c r="O43" t="s">
         <v>58</v>
       </c>
-      <c r="P43" t="s">
+      <c r="Q43" t="s">
         <v>59</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <v>4</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>49</v>
       </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>36</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <v>1</v>
       </c>
-      <c r="V43" t="s">
+      <c r="W43" t="s">
         <v>56</v>
       </c>
-      <c r="W43" t="s">
+      <c r="X43" t="s">
         <v>37</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
         <v>38</v>
       </c>
-      <c r="AB43" t="s">
+      <c r="AC43" t="s">
         <v>56</v>
       </c>
-      <c r="AC43" t="s">
+      <c r="AD43" t="s">
         <v>145</v>
       </c>
-      <c r="AD43" t="s">
+      <c r="AE43" t="s">
         <v>57</v>
       </c>
-      <c r="AE43" t="s">
+      <c r="AF43" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -3563,56 +3575,59 @@
       <c r="H44" t="s">
         <v>147</v>
       </c>
-      <c r="K44" s="3" t="s">
+      <c r="K44">
+        <v>360</v>
+      </c>
+      <c r="L44" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L44" t="s">
-        <v>60</v>
       </c>
       <c r="M44" t="s">
         <v>60</v>
       </c>
       <c r="N44" t="s">
+        <v>60</v>
+      </c>
+      <c r="O44" t="s">
         <v>61</v>
       </c>
-      <c r="O44" t="s">
+      <c r="P44" t="s">
         <v>62</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <v>5</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>49</v>
       </c>
-      <c r="S44" t="s">
+      <c r="T44" t="s">
         <v>36</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>1</v>
       </c>
-      <c r="W44" t="s">
+      <c r="X44" t="s">
         <v>37</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
         <v>38</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>39</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="AA44" t="s">
         <v>40</v>
       </c>
-      <c r="AA44" t="s">
+      <c r="AB44" t="s">
         <v>41</v>
-      </c>
-      <c r="AD44" t="s">
-        <v>60</v>
       </c>
       <c r="AE44" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -3631,41 +3646,44 @@
       <c r="H45" t="s">
         <v>147</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="K45">
+        <v>360</v>
+      </c>
+      <c r="L45" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L45" t="s">
-        <v>63</v>
       </c>
       <c r="M45" t="s">
         <v>63</v>
       </c>
       <c r="N45" t="s">
+        <v>63</v>
+      </c>
+      <c r="O45" t="s">
         <v>65</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>66</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
         <v>6</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>56</v>
       </c>
-      <c r="S45" t="s">
+      <c r="T45" t="s">
         <v>67</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>10</v>
-      </c>
-      <c r="AD45" t="s">
-        <v>64</v>
       </c>
       <c r="AE45" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>43</v>
       </c>
@@ -3684,56 +3702,59 @@
       <c r="H46" t="s">
         <v>147</v>
       </c>
-      <c r="K46" s="3" t="s">
+      <c r="K46">
+        <v>360</v>
+      </c>
+      <c r="L46" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L46" t="s">
-        <v>71</v>
       </c>
       <c r="M46" t="s">
         <v>71</v>
       </c>
       <c r="N46" t="s">
+        <v>71</v>
+      </c>
+      <c r="O46" t="s">
         <v>72</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
         <v>73</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <v>8</v>
       </c>
-      <c r="R46" t="s">
+      <c r="S46" t="s">
         <v>49</v>
       </c>
-      <c r="S46" t="s">
+      <c r="T46" t="s">
         <v>36</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <v>200</v>
       </c>
-      <c r="V46" t="s">
+      <c r="W46" t="s">
         <v>56</v>
       </c>
-      <c r="W46" t="s">
+      <c r="X46" t="s">
         <v>74</v>
       </c>
-      <c r="X46" t="s">
+      <c r="Y46" t="s">
         <v>75</v>
       </c>
-      <c r="AB46" t="s">
+      <c r="AC46" t="s">
         <v>76</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="AD46" t="s">
         <v>77</v>
       </c>
-      <c r="AD46" t="s">
+      <c r="AE46" t="s">
         <v>71</v>
       </c>
-      <c r="AE46" t="s">
+      <c r="AF46" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>78</v>
       </c>
@@ -3752,44 +3773,47 @@
       <c r="H47" t="s">
         <v>148</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K47">
+        <v>360</v>
+      </c>
+      <c r="L47" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L47" t="s">
-        <v>46</v>
       </c>
       <c r="M47" t="s">
         <v>46</v>
       </c>
       <c r="N47" t="s">
+        <v>46</v>
+      </c>
+      <c r="O47" t="s">
         <v>47</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>48</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <v>1</v>
       </c>
-      <c r="R47" t="s">
+      <c r="S47" t="s">
         <v>49</v>
       </c>
-      <c r="S47" t="s">
+      <c r="T47" t="s">
         <v>36</v>
       </c>
-      <c r="T47">
+      <c r="U47">
         <v>200</v>
       </c>
-      <c r="AB47" t="s">
+      <c r="AC47" t="s">
         <v>137</v>
       </c>
-      <c r="AD47" t="s">
+      <c r="AE47" t="s">
         <v>46</v>
       </c>
-      <c r="AE47" t="s">
+      <c r="AF47" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>78</v>
       </c>
@@ -3808,53 +3832,56 @@
       <c r="H48" t="s">
         <v>148</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="K48">
+        <v>360</v>
+      </c>
+      <c r="L48" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L48" t="s">
-        <v>53</v>
       </c>
       <c r="M48" t="s">
         <v>53</v>
       </c>
       <c r="N48" t="s">
+        <v>53</v>
+      </c>
+      <c r="O48" t="s">
         <v>54</v>
       </c>
-      <c r="P48" t="s">
+      <c r="Q48" t="s">
         <v>55</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <v>3</v>
       </c>
-      <c r="R48" t="s">
+      <c r="S48" t="s">
         <v>56</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
         <v>36</v>
       </c>
-      <c r="T48">
+      <c r="U48">
         <v>200</v>
       </c>
-      <c r="W48" t="s">
+      <c r="X48" t="s">
         <v>138</v>
       </c>
-      <c r="X48" t="s">
+      <c r="Y48" t="s">
         <v>139</v>
       </c>
-      <c r="AB48" t="s">
+      <c r="AC48" t="s">
         <v>141</v>
       </c>
-      <c r="AC48" t="s">
+      <c r="AD48" t="s">
         <v>78</v>
       </c>
-      <c r="AD48" t="s">
+      <c r="AE48" t="s">
         <v>53</v>
       </c>
-      <c r="AE48" t="s">
+      <c r="AF48" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>78</v>
       </c>
@@ -3873,56 +3900,59 @@
       <c r="H49" t="s">
         <v>148</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="K49">
+        <v>360</v>
+      </c>
+      <c r="L49" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L49" t="s">
-        <v>57</v>
       </c>
       <c r="M49" t="s">
         <v>57</v>
       </c>
       <c r="N49" t="s">
+        <v>57</v>
+      </c>
+      <c r="O49" t="s">
         <v>58</v>
       </c>
-      <c r="P49" t="s">
+      <c r="Q49" t="s">
         <v>59</v>
       </c>
-      <c r="Q49">
+      <c r="R49">
         <v>4</v>
       </c>
-      <c r="R49" t="s">
+      <c r="S49" t="s">
         <v>49</v>
       </c>
-      <c r="S49" t="s">
+      <c r="T49" t="s">
         <v>36</v>
       </c>
-      <c r="T49">
+      <c r="U49">
         <v>1</v>
       </c>
-      <c r="V49" t="s">
+      <c r="W49" t="s">
         <v>56</v>
       </c>
-      <c r="W49" t="s">
+      <c r="X49" t="s">
         <v>37</v>
       </c>
-      <c r="X49" t="s">
+      <c r="Y49" t="s">
         <v>38</v>
       </c>
-      <c r="AB49" t="s">
+      <c r="AC49" t="s">
         <v>56</v>
       </c>
-      <c r="AC49" t="s">
+      <c r="AD49" t="s">
         <v>145</v>
       </c>
-      <c r="AD49" t="s">
+      <c r="AE49" t="s">
         <v>57</v>
       </c>
-      <c r="AE49" t="s">
+      <c r="AF49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>78</v>
       </c>
@@ -3941,56 +3971,59 @@
       <c r="H50" t="s">
         <v>148</v>
       </c>
-      <c r="K50" s="3" t="s">
+      <c r="K50">
+        <v>360</v>
+      </c>
+      <c r="L50" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L50" t="s">
-        <v>60</v>
       </c>
       <c r="M50" t="s">
         <v>60</v>
       </c>
       <c r="N50" t="s">
+        <v>60</v>
+      </c>
+      <c r="O50" t="s">
         <v>61</v>
       </c>
-      <c r="O50" t="s">
+      <c r="P50" t="s">
         <v>81</v>
       </c>
-      <c r="Q50">
+      <c r="R50">
         <v>5</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>49</v>
       </c>
-      <c r="S50" t="s">
+      <c r="T50" t="s">
         <v>36</v>
       </c>
-      <c r="T50">
+      <c r="U50">
         <v>1</v>
       </c>
-      <c r="W50" t="s">
+      <c r="X50" t="s">
         <v>37</v>
       </c>
-      <c r="X50" t="s">
+      <c r="Y50" t="s">
         <v>38</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>39</v>
       </c>
-      <c r="Z50" t="s">
+      <c r="AA50" t="s">
         <v>40</v>
       </c>
-      <c r="AA50" t="s">
+      <c r="AB50" t="s">
         <v>41</v>
-      </c>
-      <c r="AD50" t="s">
-        <v>60</v>
       </c>
       <c r="AE50" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>78</v>
       </c>
@@ -4009,41 +4042,44 @@
       <c r="H51" t="s">
         <v>148</v>
       </c>
-      <c r="K51" s="3" t="s">
+      <c r="K51">
+        <v>360</v>
+      </c>
+      <c r="L51" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L51" t="s">
-        <v>63</v>
       </c>
       <c r="M51" t="s">
         <v>63</v>
       </c>
       <c r="N51" t="s">
+        <v>63</v>
+      </c>
+      <c r="O51" t="s">
         <v>65</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>66</v>
       </c>
-      <c r="Q51">
+      <c r="R51">
         <v>6</v>
       </c>
-      <c r="R51" t="s">
+      <c r="S51" t="s">
         <v>56</v>
       </c>
-      <c r="S51" t="s">
+      <c r="T51" t="s">
         <v>67</v>
       </c>
-      <c r="T51">
+      <c r="U51">
         <v>10</v>
-      </c>
-      <c r="AD51" t="s">
-        <v>64</v>
       </c>
       <c r="AE51" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>78</v>
       </c>
@@ -4062,56 +4098,59 @@
       <c r="H52" t="s">
         <v>148</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="K52">
+        <v>360</v>
+      </c>
+      <c r="L52" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="L52" t="s">
-        <v>71</v>
       </c>
       <c r="M52" t="s">
         <v>71</v>
       </c>
       <c r="N52" t="s">
+        <v>71</v>
+      </c>
+      <c r="O52" t="s">
         <v>72</v>
       </c>
-      <c r="P52" t="s">
+      <c r="Q52" t="s">
         <v>73</v>
       </c>
-      <c r="Q52">
+      <c r="R52">
         <v>8</v>
       </c>
-      <c r="R52" t="s">
+      <c r="S52" t="s">
         <v>49</v>
       </c>
-      <c r="S52" t="s">
+      <c r="T52" t="s">
         <v>36</v>
       </c>
-      <c r="T52">
+      <c r="U52">
         <v>200</v>
       </c>
-      <c r="V52" t="s">
+      <c r="W52" t="s">
         <v>56</v>
       </c>
-      <c r="W52" t="s">
+      <c r="X52" t="s">
         <v>74</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Y52" t="s">
         <v>75</v>
       </c>
-      <c r="AB52" t="s">
+      <c r="AC52" t="s">
         <v>82</v>
       </c>
-      <c r="AC52" t="s">
+      <c r="AD52" t="s">
         <v>83</v>
       </c>
-      <c r="AD52" t="s">
+      <c r="AE52" t="s">
         <v>71</v>
       </c>
-      <c r="AE52" t="s">
+      <c r="AF52" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>84</v>
       </c>
@@ -4130,44 +4169,47 @@
       <c r="H53" t="s">
         <v>149</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53">
+        <v>360</v>
+      </c>
+      <c r="L53" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L53" t="s">
-        <v>46</v>
       </c>
       <c r="M53" t="s">
         <v>46</v>
       </c>
       <c r="N53" t="s">
+        <v>46</v>
+      </c>
+      <c r="O53" t="s">
         <v>47</v>
       </c>
-      <c r="P53" t="s">
+      <c r="Q53" t="s">
         <v>48</v>
       </c>
-      <c r="Q53">
+      <c r="R53">
         <v>1</v>
       </c>
-      <c r="R53" t="s">
+      <c r="S53" t="s">
         <v>49</v>
       </c>
-      <c r="S53" t="s">
+      <c r="T53" t="s">
         <v>36</v>
       </c>
-      <c r="T53">
+      <c r="U53">
         <v>200</v>
       </c>
-      <c r="AB53" t="s">
+      <c r="AC53" t="s">
         <v>137</v>
       </c>
-      <c r="AD53" t="s">
+      <c r="AE53" t="s">
         <v>46</v>
       </c>
-      <c r="AE53" t="s">
+      <c r="AF53" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>84</v>
       </c>
@@ -4186,53 +4228,56 @@
       <c r="H54" t="s">
         <v>149</v>
       </c>
-      <c r="K54" s="3" t="s">
+      <c r="K54">
+        <v>360</v>
+      </c>
+      <c r="L54" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L54" t="s">
-        <v>53</v>
       </c>
       <c r="M54" t="s">
         <v>53</v>
       </c>
       <c r="N54" t="s">
+        <v>53</v>
+      </c>
+      <c r="O54" t="s">
         <v>54</v>
       </c>
-      <c r="P54" t="s">
+      <c r="Q54" t="s">
         <v>55</v>
       </c>
-      <c r="Q54">
+      <c r="R54">
         <v>3</v>
       </c>
-      <c r="R54" t="s">
+      <c r="S54" t="s">
         <v>56</v>
       </c>
-      <c r="S54" t="s">
+      <c r="T54" t="s">
         <v>36</v>
       </c>
-      <c r="T54">
+      <c r="U54">
         <v>200</v>
       </c>
-      <c r="W54" t="s">
+      <c r="X54" t="s">
         <v>138</v>
       </c>
-      <c r="X54" t="s">
+      <c r="Y54" t="s">
         <v>139</v>
       </c>
-      <c r="AB54" s="6" t="s">
+      <c r="AC54" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="AC54" s="6" t="s">
+      <c r="AD54" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AD54" t="s">
+      <c r="AE54" t="s">
         <v>53</v>
       </c>
-      <c r="AE54" t="s">
+      <c r="AF54" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>84</v>
       </c>
@@ -4251,56 +4296,59 @@
       <c r="H55" t="s">
         <v>149</v>
       </c>
-      <c r="K55" s="3" t="s">
+      <c r="K55">
+        <v>360</v>
+      </c>
+      <c r="L55" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L55" t="s">
-        <v>57</v>
       </c>
       <c r="M55" t="s">
         <v>57</v>
       </c>
       <c r="N55" t="s">
+        <v>57</v>
+      </c>
+      <c r="O55" t="s">
         <v>58</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>59</v>
       </c>
-      <c r="Q55">
+      <c r="R55">
         <v>4</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>49</v>
       </c>
-      <c r="S55" t="s">
+      <c r="T55" t="s">
         <v>36</v>
       </c>
-      <c r="T55">
+      <c r="U55">
         <v>1</v>
       </c>
-      <c r="V55" t="s">
+      <c r="W55" t="s">
         <v>56</v>
       </c>
-      <c r="W55" t="s">
+      <c r="X55" t="s">
         <v>37</v>
       </c>
-      <c r="X55" t="s">
+      <c r="Y55" t="s">
         <v>38</v>
       </c>
-      <c r="AB55" t="s">
+      <c r="AC55" t="s">
         <v>56</v>
       </c>
-      <c r="AC55" t="s">
+      <c r="AD55" t="s">
         <v>145</v>
       </c>
-      <c r="AD55" t="s">
+      <c r="AE55" t="s">
         <v>57</v>
       </c>
-      <c r="AE55" t="s">
+      <c r="AF55" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>84</v>
       </c>
@@ -4319,56 +4367,59 @@
       <c r="H56" t="s">
         <v>149</v>
       </c>
-      <c r="K56" s="3" t="s">
+      <c r="K56">
+        <v>360</v>
+      </c>
+      <c r="L56" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L56" t="s">
-        <v>60</v>
       </c>
       <c r="M56" t="s">
         <v>60</v>
       </c>
       <c r="N56" t="s">
+        <v>60</v>
+      </c>
+      <c r="O56" t="s">
         <v>61</v>
       </c>
-      <c r="O56" t="s">
+      <c r="P56" t="s">
         <v>87</v>
       </c>
-      <c r="Q56">
+      <c r="R56">
         <v>5</v>
       </c>
-      <c r="R56" t="s">
+      <c r="S56" t="s">
         <v>49</v>
       </c>
-      <c r="S56" t="s">
+      <c r="T56" t="s">
         <v>36</v>
       </c>
-      <c r="T56">
+      <c r="U56">
         <v>1</v>
       </c>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>37</v>
       </c>
-      <c r="X56" t="s">
+      <c r="Y56" t="s">
         <v>38</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>39</v>
       </c>
-      <c r="Z56" t="s">
+      <c r="AA56" t="s">
         <v>40</v>
       </c>
-      <c r="AA56" t="s">
+      <c r="AB56" t="s">
         <v>41</v>
-      </c>
-      <c r="AD56" t="s">
-        <v>60</v>
       </c>
       <c r="AE56" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>84</v>
       </c>
@@ -4387,41 +4438,44 @@
       <c r="H57" t="s">
         <v>149</v>
       </c>
-      <c r="K57" s="3" t="s">
+      <c r="K57">
+        <v>360</v>
+      </c>
+      <c r="L57" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L57" t="s">
-        <v>63</v>
       </c>
       <c r="M57" t="s">
         <v>63</v>
       </c>
       <c r="N57" t="s">
+        <v>63</v>
+      </c>
+      <c r="O57" t="s">
         <v>65</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
         <v>66</v>
       </c>
-      <c r="Q57">
+      <c r="R57">
         <v>6</v>
       </c>
-      <c r="R57" t="s">
+      <c r="S57" t="s">
         <v>56</v>
       </c>
-      <c r="S57" t="s">
+      <c r="T57" t="s">
         <v>67</v>
       </c>
-      <c r="T57">
+      <c r="U57">
         <v>10</v>
-      </c>
-      <c r="AD57" t="s">
-        <v>64</v>
       </c>
       <c r="AE57" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="58" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>84</v>
       </c>
@@ -4440,56 +4494,59 @@
       <c r="H58" t="s">
         <v>149</v>
       </c>
-      <c r="K58" s="3" t="s">
+      <c r="K58">
+        <v>360</v>
+      </c>
+      <c r="L58" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L58" t="s">
-        <v>71</v>
       </c>
       <c r="M58" t="s">
         <v>71</v>
       </c>
       <c r="N58" t="s">
+        <v>71</v>
+      </c>
+      <c r="O58" t="s">
         <v>72</v>
       </c>
-      <c r="P58" t="s">
+      <c r="Q58" t="s">
         <v>73</v>
       </c>
-      <c r="Q58">
+      <c r="R58">
         <v>8</v>
       </c>
-      <c r="R58" t="s">
+      <c r="S58" t="s">
         <v>49</v>
       </c>
-      <c r="S58" t="s">
+      <c r="T58" t="s">
         <v>36</v>
       </c>
-      <c r="T58">
+      <c r="U58">
         <v>200</v>
       </c>
-      <c r="V58" t="s">
+      <c r="W58" t="s">
         <v>56</v>
       </c>
-      <c r="W58" t="s">
+      <c r="X58" t="s">
         <v>74</v>
       </c>
-      <c r="X58" t="s">
+      <c r="Y58" t="s">
         <v>75</v>
       </c>
-      <c r="AB58" t="s">
+      <c r="AC58" t="s">
         <v>76</v>
       </c>
-      <c r="AC58" t="s">
+      <c r="AD58" t="s">
         <v>77</v>
       </c>
-      <c r="AD58" t="s">
+      <c r="AE58" t="s">
         <v>71</v>
       </c>
-      <c r="AE58" t="s">
+      <c r="AF58" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>150</v>
       </c>
@@ -4505,47 +4562,50 @@
       <c r="H59" t="s">
         <v>154</v>
       </c>
-      <c r="K59" s="3" t="s">
+      <c r="K59">
+        <v>360</v>
+      </c>
+      <c r="L59" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="L59" t="s">
-        <v>34</v>
       </c>
       <c r="M59" t="s">
         <v>34</v>
       </c>
-      <c r="O59" t="s">
+      <c r="N59" t="s">
+        <v>34</v>
+      </c>
+      <c r="P59" t="s">
         <v>35</v>
       </c>
-      <c r="Q59">
+      <c r="R59">
         <v>1</v>
       </c>
-      <c r="S59" t="s">
+      <c r="T59" t="s">
         <v>36</v>
       </c>
-      <c r="T59">
+      <c r="U59">
         <v>1</v>
       </c>
-      <c r="W59" t="s">
+      <c r="X59" t="s">
         <v>37</v>
       </c>
-      <c r="X59" t="s">
+      <c r="Y59" t="s">
         <v>38</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>39</v>
       </c>
-      <c r="Z59" t="s">
+      <c r="AA59" t="s">
         <v>40</v>
       </c>
-      <c r="AA59" t="s">
+      <c r="AB59" t="s">
         <v>41</v>
       </c>
-      <c r="AE59" t="s">
+      <c r="AF59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:32" ht="32" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>150</v>
       </c>
@@ -4559,53 +4619,53 @@
         <v>33</v>
       </c>
       <c r="H60" t="s">
-        <v>157</v>
-      </c>
-      <c r="J60" t="s">
-        <v>155</v>
-      </c>
-      <c r="K60" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K60">
+        <v>360</v>
+      </c>
+      <c r="L60" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="L60" t="s">
-        <v>34</v>
       </c>
       <c r="M60" t="s">
         <v>34</v>
       </c>
-      <c r="P60" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q60">
+      <c r="N60" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>155</v>
+      </c>
+      <c r="R60">
         <v>1</v>
       </c>
-      <c r="S60" t="s">
+      <c r="T60" t="s">
         <v>36</v>
       </c>
-      <c r="T60">
+      <c r="U60">
         <v>1</v>
       </c>
-      <c r="W60" t="s">
+      <c r="X60" t="s">
         <v>37</v>
       </c>
-      <c r="X60" t="s">
+      <c r="Y60" t="s">
         <v>38</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>39</v>
       </c>
-      <c r="Z60" t="s">
+      <c r="AA60" t="s">
         <v>40</v>
       </c>
-      <c r="AA60" t="s">
+      <c r="AB60" t="s">
         <v>41</v>
       </c>
-      <c r="AE60" t="s">
+      <c r="AF60" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI60" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ60" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added derivation columns (blank) - PR
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_PR.xlsx
+++ b/curation/draft/collection/collection_specialization_PR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F53AE-2878-F749-ABC2-8D2ECFE7D296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA6272B-587E-2E4E-83FA-C7293BC17170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Collection_PR" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_PR!$A$1:$AJ$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_PR!$A$1:$AL$60</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="160">
   <si>
     <t>package_date</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -879,12 +885,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH60"/>
+  <dimension ref="A1:AJ60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -898,14 +904,14 @@
     <col min="16" max="16" width="32.1640625" customWidth="1"/>
     <col min="17" max="17" width="21" customWidth="1"/>
     <col min="18" max="18" width="12.33203125" customWidth="1"/>
-    <col min="26" max="26" width="19.83203125" customWidth="1"/>
-    <col min="27" max="27" width="14.83203125" customWidth="1"/>
-    <col min="29" max="29" width="17" customWidth="1"/>
-    <col min="30" max="30" width="13.33203125" customWidth="1"/>
-    <col min="32" max="32" width="22.1640625" customWidth="1"/>
+    <col min="28" max="28" width="19.83203125" customWidth="1"/>
+    <col min="29" max="29" width="14.83203125" customWidth="1"/>
+    <col min="31" max="31" width="17" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" customWidth="1"/>
+    <col min="34" max="34" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,40 +982,46 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>150</v>
       </c>
@@ -1046,26 +1058,26 @@
       <c r="U2">
         <v>1</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>40</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>41</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>150</v>
       </c>
@@ -1102,14 +1114,14 @@
       <c r="U3">
         <v>10</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>153</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>43</v>
       </c>
@@ -1155,17 +1167,17 @@
       <c r="U4">
         <v>200</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
         <v>137</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>46</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -1211,14 +1223,14 @@
       <c r="U5">
         <v>200</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>50</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>43</v>
       </c>
@@ -1264,26 +1276,26 @@
       <c r="U6">
         <v>200</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>138</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>139</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AE6" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AF6" t="s">
         <v>43</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>53</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>43</v>
       </c>
@@ -1332,26 +1344,26 @@
       <c r="W7" t="s">
         <v>56</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>37</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>56</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AF7" t="s">
         <v>145</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>57</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1397,29 +1409,29 @@
       <c r="U8">
         <v>1</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>37</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>38</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB8" t="s">
         <v>39</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AC8" t="s">
         <v>40</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AD8" t="s">
         <v>41</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>60</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>43</v>
       </c>
@@ -1465,14 +1477,14 @@
       <c r="U9">
         <v>10</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AG9" t="s">
         <v>64</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -1518,14 +1530,14 @@
       <c r="U10">
         <v>5</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" t="s">
         <v>64</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -1574,26 +1586,26 @@
       <c r="W11" t="s">
         <v>56</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA11" t="s">
         <v>75</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AE11" t="s">
         <v>76</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AF11" t="s">
         <v>77</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AG11" t="s">
         <v>71</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>78</v>
       </c>
@@ -1639,17 +1651,17 @@
       <c r="U12">
         <v>200</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AE12" t="s">
         <v>137</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>46</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>78</v>
       </c>
@@ -1695,14 +1707,14 @@
       <c r="U13">
         <v>200</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>50</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>78</v>
       </c>
@@ -1748,26 +1760,26 @@
       <c r="U14">
         <v>200</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Z14" t="s">
         <v>138</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>139</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AE14" t="s">
         <v>141</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AF14" t="s">
         <v>78</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>53</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>78</v>
       </c>
@@ -1816,26 +1828,26 @@
       <c r="W15" t="s">
         <v>56</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Z15" t="s">
         <v>37</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AA15" t="s">
         <v>38</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AE15" t="s">
         <v>56</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AF15" t="s">
         <v>145</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AG15" t="s">
         <v>57</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AH15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>78</v>
       </c>
@@ -1881,29 +1893,29 @@
       <c r="U16">
         <v>1</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Z16" t="s">
         <v>37</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AA16" t="s">
         <v>38</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AB16" t="s">
         <v>39</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AC16" t="s">
         <v>40</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
         <v>41</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>60</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AH16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>78</v>
       </c>
@@ -1949,14 +1961,14 @@
       <c r="U17">
         <v>10</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AG17" t="s">
         <v>64</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AH17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>78</v>
       </c>
@@ -2002,14 +2014,14 @@
       <c r="U18">
         <v>5</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AG18" t="s">
         <v>64</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AH18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>78</v>
       </c>
@@ -2058,26 +2070,26 @@
       <c r="W19" t="s">
         <v>56</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Z19" t="s">
         <v>74</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="AA19" t="s">
         <v>75</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AE19" t="s">
         <v>82</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AF19" t="s">
         <v>83</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AG19" t="s">
         <v>71</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AH19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>84</v>
       </c>
@@ -2123,17 +2135,17 @@
       <c r="U20">
         <v>200</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AE20" t="s">
         <v>137</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AG20" t="s">
         <v>46</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AH20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>84</v>
       </c>
@@ -2179,14 +2191,14 @@
       <c r="U21">
         <v>200</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AG21" t="s">
         <v>50</v>
       </c>
-      <c r="AF21" t="s">
+      <c r="AH21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>84</v>
       </c>
@@ -2232,26 +2244,26 @@
       <c r="U22">
         <v>200</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Z22" t="s">
         <v>138</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="AA22" t="s">
         <v>139</v>
       </c>
-      <c r="AC22" s="6" t="s">
+      <c r="AE22" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="AD22" s="6" t="s">
+      <c r="AF22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AG22" t="s">
         <v>53</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AH22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>84</v>
       </c>
@@ -2300,26 +2312,26 @@
       <c r="W23" t="s">
         <v>56</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Z23" t="s">
         <v>37</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="AA23" t="s">
         <v>38</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AE23" t="s">
         <v>56</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AF23" t="s">
         <v>145</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AG23" t="s">
         <v>57</v>
       </c>
-      <c r="AF23" t="s">
+      <c r="AH23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -2365,29 +2377,29 @@
       <c r="U24">
         <v>1</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Z24" t="s">
         <v>37</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="AA24" t="s">
         <v>38</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AB24" t="s">
         <v>39</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AC24" t="s">
         <v>40</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AD24" t="s">
         <v>41</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AG24" t="s">
         <v>60</v>
       </c>
-      <c r="AF24" t="s">
+      <c r="AH24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>84</v>
       </c>
@@ -2433,14 +2445,14 @@
       <c r="U25">
         <v>10</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AG25" t="s">
         <v>64</v>
       </c>
-      <c r="AF25" t="s">
+      <c r="AH25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>84</v>
       </c>
@@ -2486,14 +2498,14 @@
       <c r="U26">
         <v>5</v>
       </c>
-      <c r="AE26" t="s">
+      <c r="AG26" t="s">
         <v>64</v>
       </c>
-      <c r="AF26" t="s">
+      <c r="AH26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>84</v>
       </c>
@@ -2542,26 +2554,26 @@
       <c r="W27" t="s">
         <v>56</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Z27" t="s">
         <v>74</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="AA27" t="s">
         <v>75</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AE27" t="s">
         <v>76</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AF27" t="s">
         <v>77</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AG27" t="s">
         <v>71</v>
       </c>
-      <c r="AF27" t="s">
+      <c r="AH27" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>88</v>
       </c>
@@ -2607,17 +2619,17 @@
       <c r="U28">
         <v>200</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="AE28" t="s">
         <v>91</v>
       </c>
-      <c r="AE28" t="s">
+      <c r="AG28" t="s">
         <v>46</v>
       </c>
-      <c r="AF28" t="s">
+      <c r="AH28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>88</v>
       </c>
@@ -2663,23 +2675,23 @@
       <c r="U29">
         <v>200</v>
       </c>
-      <c r="Z29" t="s">
+      <c r="AB29" t="s">
         <v>92</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AC29" t="s">
         <v>93</v>
       </c>
-      <c r="AB29" t="s">
+      <c r="AD29" t="s">
         <v>41</v>
       </c>
-      <c r="AE29" t="s">
+      <c r="AG29" t="s">
         <v>50</v>
       </c>
-      <c r="AF29" t="s">
+      <c r="AH29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>88</v>
       </c>
@@ -2725,17 +2737,17 @@
       <c r="U30">
         <v>200</v>
       </c>
-      <c r="AC30" t="s">
+      <c r="AE30" t="s">
         <v>97</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AG30" t="s">
         <v>94</v>
       </c>
-      <c r="AF30" t="s">
+      <c r="AH30" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>88</v>
       </c>
@@ -2781,29 +2793,29 @@
       <c r="U31">
         <v>200</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Z31" t="s">
         <v>138</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="AA31" t="s">
         <v>139</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="AB31" t="s">
         <v>98</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AC31" t="s">
         <v>99</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AD31" t="s">
         <v>41</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AG31" t="s">
         <v>53</v>
       </c>
-      <c r="AF31" t="s">
+      <c r="AH31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>88</v>
       </c>
@@ -2849,29 +2861,29 @@
       <c r="U32">
         <v>200</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Z32" t="s">
         <v>103</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="AA32" t="s">
         <v>104</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AB32" t="s">
         <v>105</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AC32" t="s">
         <v>106</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AD32" t="s">
         <v>41</v>
       </c>
-      <c r="AE32" t="s">
+      <c r="AG32" t="s">
         <v>100</v>
       </c>
-      <c r="AF32" t="s">
+      <c r="AH32" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>88</v>
       </c>
@@ -2917,29 +2929,29 @@
       <c r="U33">
         <v>200</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Z33" t="s">
         <v>111</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="AA33" t="s">
         <v>112</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="AB33" t="s">
         <v>113</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="AC33" t="s">
         <v>114</v>
       </c>
-      <c r="AB33" t="s">
+      <c r="AD33" t="s">
         <v>41</v>
       </c>
-      <c r="AE33" t="s">
+      <c r="AG33" t="s">
         <v>108</v>
       </c>
-      <c r="AF33" t="s">
+      <c r="AH33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>88</v>
       </c>
@@ -2988,26 +3000,26 @@
       <c r="W34" t="s">
         <v>56</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Z34" t="s">
         <v>37</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="AA34" t="s">
         <v>38</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AE34" t="s">
         <v>56</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AF34" t="s">
         <v>145</v>
       </c>
-      <c r="AE34" t="s">
+      <c r="AG34" t="s">
         <v>57</v>
       </c>
-      <c r="AF34" t="s">
+      <c r="AH34" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>88</v>
       </c>
@@ -3053,29 +3065,29 @@
       <c r="U35">
         <v>1</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Z35" t="s">
         <v>37</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="AA35" t="s">
         <v>38</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="AB35" t="s">
         <v>39</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AC35" t="s">
         <v>40</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AD35" t="s">
         <v>41</v>
       </c>
-      <c r="AE35" t="s">
+      <c r="AG35" t="s">
         <v>60</v>
       </c>
-      <c r="AF35" t="s">
+      <c r="AH35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>88</v>
       </c>
@@ -3121,14 +3133,14 @@
       <c r="U36">
         <v>10</v>
       </c>
-      <c r="AE36" t="s">
+      <c r="AG36" t="s">
         <v>64</v>
       </c>
-      <c r="AF36" t="s">
+      <c r="AH36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -3171,14 +3183,14 @@
       <c r="U37">
         <v>100</v>
       </c>
-      <c r="AE37" t="s">
+      <c r="AG37" t="s">
         <v>119</v>
       </c>
-      <c r="AF37" t="s">
+      <c r="AH37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>88</v>
       </c>
@@ -3224,20 +3236,20 @@
       <c r="U38">
         <v>20</v>
       </c>
-      <c r="AC38" t="s">
+      <c r="AE38" t="s">
         <v>123</v>
       </c>
-      <c r="AD38" t="s">
+      <c r="AF38" t="s">
         <v>124</v>
       </c>
-      <c r="AE38" t="s">
+      <c r="AG38" t="s">
         <v>120</v>
       </c>
-      <c r="AF38" t="s">
+      <c r="AH38" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>88</v>
       </c>
@@ -3283,14 +3295,14 @@
       <c r="U39">
         <v>5</v>
       </c>
-      <c r="AE39" t="s">
+      <c r="AG39" t="s">
         <v>64</v>
       </c>
-      <c r="AF39" t="s">
+      <c r="AH39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -3336,29 +3348,29 @@
       <c r="U40">
         <v>20</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Z40" t="s">
         <v>74</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="AA40" t="s">
         <v>75</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="AB40" t="s">
         <v>125</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AC40" t="s">
         <v>126</v>
       </c>
-      <c r="AB40" t="s">
+      <c r="AD40" t="s">
         <v>41</v>
       </c>
-      <c r="AE40" t="s">
+      <c r="AG40" t="s">
         <v>71</v>
       </c>
-      <c r="AF40" t="s">
+      <c r="AH40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -3407,17 +3419,17 @@
       <c r="U41">
         <v>200</v>
       </c>
-      <c r="AC41" t="s">
+      <c r="AE41" t="s">
         <v>137</v>
       </c>
-      <c r="AE41" t="s">
+      <c r="AG41" t="s">
         <v>46</v>
       </c>
-      <c r="AF41" t="s">
+      <c r="AH41" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>43</v>
       </c>
@@ -3466,26 +3478,26 @@
       <c r="U42">
         <v>200</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Z42" t="s">
         <v>138</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="AA42" t="s">
         <v>139</v>
       </c>
-      <c r="AC42" s="6" t="s">
+      <c r="AE42" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AF42" t="s">
         <v>43</v>
       </c>
-      <c r="AE42" t="s">
+      <c r="AG42" t="s">
         <v>53</v>
       </c>
-      <c r="AF42" t="s">
+      <c r="AH42" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>43</v>
       </c>
@@ -3537,26 +3549,26 @@
       <c r="W43" t="s">
         <v>56</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Z43" t="s">
         <v>37</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="AA43" t="s">
         <v>38</v>
       </c>
-      <c r="AC43" t="s">
+      <c r="AE43" t="s">
         <v>56</v>
       </c>
-      <c r="AD43" t="s">
+      <c r="AF43" t="s">
         <v>145</v>
       </c>
-      <c r="AE43" t="s">
+      <c r="AG43" t="s">
         <v>57</v>
       </c>
-      <c r="AF43" t="s">
+      <c r="AH43" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -3605,29 +3617,29 @@
       <c r="U44">
         <v>1</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Z44" t="s">
         <v>37</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="AA44" t="s">
         <v>38</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="AB44" t="s">
         <v>39</v>
       </c>
-      <c r="AA44" t="s">
+      <c r="AC44" t="s">
         <v>40</v>
       </c>
-      <c r="AB44" t="s">
+      <c r="AD44" t="s">
         <v>41</v>
       </c>
-      <c r="AE44" t="s">
+      <c r="AG44" t="s">
         <v>60</v>
       </c>
-      <c r="AF44" t="s">
+      <c r="AH44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -3676,14 +3688,14 @@
       <c r="U45">
         <v>10</v>
       </c>
-      <c r="AE45" t="s">
+      <c r="AG45" t="s">
         <v>64</v>
       </c>
-      <c r="AF45" t="s">
+      <c r="AH45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>43</v>
       </c>
@@ -3735,26 +3747,26 @@
       <c r="W46" t="s">
         <v>56</v>
       </c>
-      <c r="X46" t="s">
+      <c r="Z46" t="s">
         <v>74</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="AA46" t="s">
         <v>75</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="AE46" t="s">
         <v>76</v>
       </c>
-      <c r="AD46" t="s">
+      <c r="AF46" t="s">
         <v>77</v>
       </c>
-      <c r="AE46" t="s">
+      <c r="AG46" t="s">
         <v>71</v>
       </c>
-      <c r="AF46" t="s">
+      <c r="AH46" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>78</v>
       </c>
@@ -3803,17 +3815,17 @@
       <c r="U47">
         <v>200</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="AE47" t="s">
         <v>137</v>
       </c>
-      <c r="AE47" t="s">
+      <c r="AG47" t="s">
         <v>46</v>
       </c>
-      <c r="AF47" t="s">
+      <c r="AH47" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>78</v>
       </c>
@@ -3862,26 +3874,26 @@
       <c r="U48">
         <v>200</v>
       </c>
-      <c r="X48" t="s">
+      <c r="Z48" t="s">
         <v>138</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="AA48" t="s">
         <v>139</v>
       </c>
-      <c r="AC48" t="s">
+      <c r="AE48" t="s">
         <v>141</v>
       </c>
-      <c r="AD48" t="s">
+      <c r="AF48" t="s">
         <v>78</v>
       </c>
-      <c r="AE48" t="s">
+      <c r="AG48" t="s">
         <v>53</v>
       </c>
-      <c r="AF48" t="s">
+      <c r="AH48" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>78</v>
       </c>
@@ -3933,26 +3945,26 @@
       <c r="W49" t="s">
         <v>56</v>
       </c>
-      <c r="X49" t="s">
+      <c r="Z49" t="s">
         <v>37</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="AA49" t="s">
         <v>38</v>
       </c>
-      <c r="AC49" t="s">
+      <c r="AE49" t="s">
         <v>56</v>
       </c>
-      <c r="AD49" t="s">
+      <c r="AF49" t="s">
         <v>145</v>
       </c>
-      <c r="AE49" t="s">
+      <c r="AG49" t="s">
         <v>57</v>
       </c>
-      <c r="AF49" t="s">
+      <c r="AH49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>78</v>
       </c>
@@ -4001,29 +4013,29 @@
       <c r="U50">
         <v>1</v>
       </c>
-      <c r="X50" t="s">
+      <c r="Z50" t="s">
         <v>37</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="AA50" t="s">
         <v>38</v>
       </c>
-      <c r="Z50" t="s">
+      <c r="AB50" t="s">
         <v>39</v>
       </c>
-      <c r="AA50" t="s">
+      <c r="AC50" t="s">
         <v>40</v>
       </c>
-      <c r="AB50" t="s">
+      <c r="AD50" t="s">
         <v>41</v>
       </c>
-      <c r="AE50" t="s">
+      <c r="AG50" t="s">
         <v>60</v>
       </c>
-      <c r="AF50" t="s">
+      <c r="AH50" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>78</v>
       </c>
@@ -4072,14 +4084,14 @@
       <c r="U51">
         <v>10</v>
       </c>
-      <c r="AE51" t="s">
+      <c r="AG51" t="s">
         <v>64</v>
       </c>
-      <c r="AF51" t="s">
+      <c r="AH51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>78</v>
       </c>
@@ -4131,26 +4143,26 @@
       <c r="W52" t="s">
         <v>56</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Z52" t="s">
         <v>74</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="AA52" t="s">
         <v>75</v>
       </c>
-      <c r="AC52" t="s">
+      <c r="AE52" t="s">
         <v>82</v>
       </c>
-      <c r="AD52" t="s">
+      <c r="AF52" t="s">
         <v>83</v>
       </c>
-      <c r="AE52" t="s">
+      <c r="AG52" t="s">
         <v>71</v>
       </c>
-      <c r="AF52" t="s">
+      <c r="AH52" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>84</v>
       </c>
@@ -4199,17 +4211,17 @@
       <c r="U53">
         <v>200</v>
       </c>
-      <c r="AC53" t="s">
+      <c r="AE53" t="s">
         <v>137</v>
       </c>
-      <c r="AE53" t="s">
+      <c r="AG53" t="s">
         <v>46</v>
       </c>
-      <c r="AF53" t="s">
+      <c r="AH53" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>84</v>
       </c>
@@ -4258,26 +4270,26 @@
       <c r="U54">
         <v>200</v>
       </c>
-      <c r="X54" t="s">
+      <c r="Z54" t="s">
         <v>138</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="AA54" t="s">
         <v>139</v>
       </c>
-      <c r="AC54" s="6" t="s">
+      <c r="AE54" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="AD54" s="6" t="s">
+      <c r="AF54" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AE54" t="s">
+      <c r="AG54" t="s">
         <v>53</v>
       </c>
-      <c r="AF54" t="s">
+      <c r="AH54" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>84</v>
       </c>
@@ -4329,26 +4341,26 @@
       <c r="W55" t="s">
         <v>56</v>
       </c>
-      <c r="X55" t="s">
+      <c r="Z55" t="s">
         <v>37</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="AA55" t="s">
         <v>38</v>
       </c>
-      <c r="AC55" t="s">
+      <c r="AE55" t="s">
         <v>56</v>
       </c>
-      <c r="AD55" t="s">
+      <c r="AF55" t="s">
         <v>145</v>
       </c>
-      <c r="AE55" t="s">
+      <c r="AG55" t="s">
         <v>57</v>
       </c>
-      <c r="AF55" t="s">
+      <c r="AH55" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>84</v>
       </c>
@@ -4397,29 +4409,29 @@
       <c r="U56">
         <v>1</v>
       </c>
-      <c r="X56" t="s">
+      <c r="Z56" t="s">
         <v>37</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="AA56" t="s">
         <v>38</v>
       </c>
-      <c r="Z56" t="s">
+      <c r="AB56" t="s">
         <v>39</v>
       </c>
-      <c r="AA56" t="s">
+      <c r="AC56" t="s">
         <v>40</v>
       </c>
-      <c r="AB56" t="s">
+      <c r="AD56" t="s">
         <v>41</v>
       </c>
-      <c r="AE56" t="s">
+      <c r="AG56" t="s">
         <v>60</v>
       </c>
-      <c r="AF56" t="s">
+      <c r="AH56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>84</v>
       </c>
@@ -4468,14 +4480,14 @@
       <c r="U57">
         <v>10</v>
       </c>
-      <c r="AE57" t="s">
+      <c r="AG57" t="s">
         <v>64</v>
       </c>
-      <c r="AF57" t="s">
+      <c r="AH57" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>84</v>
       </c>
@@ -4527,26 +4539,26 @@
       <c r="W58" t="s">
         <v>56</v>
       </c>
-      <c r="X58" t="s">
+      <c r="Z58" t="s">
         <v>74</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="AA58" t="s">
         <v>75</v>
       </c>
-      <c r="AC58" t="s">
+      <c r="AE58" t="s">
         <v>76</v>
       </c>
-      <c r="AD58" t="s">
+      <c r="AF58" t="s">
         <v>77</v>
       </c>
-      <c r="AE58" t="s">
+      <c r="AG58" t="s">
         <v>71</v>
       </c>
-      <c r="AF58" t="s">
+      <c r="AH58" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>150</v>
       </c>
@@ -4586,26 +4598,26 @@
       <c r="U59">
         <v>1</v>
       </c>
-      <c r="X59" t="s">
+      <c r="Z59" t="s">
         <v>37</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="AA59" t="s">
         <v>38</v>
       </c>
-      <c r="Z59" t="s">
+      <c r="AB59" t="s">
         <v>39</v>
       </c>
-      <c r="AA59" t="s">
+      <c r="AC59" t="s">
         <v>40</v>
       </c>
-      <c r="AB59" t="s">
+      <c r="AD59" t="s">
         <v>41</v>
       </c>
-      <c r="AF59" t="s">
+      <c r="AH59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>150</v>
       </c>
@@ -4645,27 +4657,27 @@
       <c r="U60">
         <v>1</v>
       </c>
-      <c r="X60" t="s">
+      <c r="Z60" t="s">
         <v>37</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="AA60" t="s">
         <v>38</v>
       </c>
-      <c r="Z60" t="s">
+      <c r="AB60" t="s">
         <v>39</v>
       </c>
-      <c r="AA60" t="s">
+      <c r="AC60" t="s">
         <v>40</v>
       </c>
-      <c r="AB60" t="s">
+      <c r="AD60" t="s">
         <v>41</v>
       </c>
-      <c r="AF60" t="s">
+      <c r="AH60" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ60" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AL60" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the bc_id for --DAT and --YN
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_PR.xlsx
+++ b/curation/draft/collection/collection_specialization_PR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA6272B-587E-2E4E-83FA-C7293BC17170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F524443F-38A9-D141-8A84-EEE7C9F389ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4000" yWindow="1940" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_PR" sheetId="1" r:id="rId1"/>
@@ -475,9 +475,6 @@
     <t>XRAYCHEST_SHORT</t>
   </si>
   <si>
-    <t>C87885</t>
-  </si>
-  <si>
     <t>PRDAT</t>
   </si>
   <si>
@@ -503,6 +500,9 @@
   </si>
   <si>
     <t>derivation_description</t>
+  </si>
+  <si>
+    <t>NEW_3</t>
   </si>
 </sst>
 </file>
@@ -887,10 +887,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="X3" sqref="X3"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -943,7 +943,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>10</v>
@@ -982,10 +982,10 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>22</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>128</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="3" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
         <v>128</v>
@@ -1097,13 +1097,13 @@
         <v>127</v>
       </c>
       <c r="M3" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q3" t="s">
         <v>151</v>
-      </c>
-      <c r="N3" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>152</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="AG3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AH3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="16" x14ac:dyDescent="0.2">
@@ -4560,7 +4560,7 @@
     </row>
     <row r="59" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D59" t="s">
         <v>128</v>
@@ -4572,7 +4572,7 @@
         <v>33</v>
       </c>
       <c r="H59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K59">
         <v>360</v>
@@ -4619,7 +4619,7 @@
     </row>
     <row r="60" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D60" t="s">
         <v>128</v>
@@ -4631,7 +4631,7 @@
         <v>33</v>
       </c>
       <c r="H60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K60">
         <v>360</v>
@@ -4646,7 +4646,7 @@
         <v>34</v>
       </c>
       <c r="Q60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R60">
         <v>1</v>

</xml_diff>